<commit_message>
RankToGodV2.1 fixed Valuation bug
</commit_message>
<xml_diff>
--- a/stocks.xlsx
+++ b/stocks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\itayt\Documents\Programming\RankToGod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE52067-BFB1-4F28-92A7-AF3B6A0972C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9693AD-9E7C-4A49-97D3-D8DDC5621125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{53EBDCE9-DC90-442D-9DEA-70CDC5EE881F}"/>
+    <workbookView xWindow="28680" yWindow="-5970" windowWidth="29040" windowHeight="15720" xr2:uid="{53EBDCE9-DC90-442D-9DEA-70CDC5EE881F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
     <t>CRHKY</t>
   </si>
   <si>
-    <t>META</t>
+    <t>V</t>
   </si>
 </sst>
 </file>
@@ -59,12 +59,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -79,8 +85,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,7 +405,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -414,7 +421,7 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updates in the readme version 2.31
</commit_message>
<xml_diff>
--- a/stocks.xlsx
+++ b/stocks.xlsx
@@ -14,27 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>symbol</t>
   </si>
   <si>
-    <t>DIS</t>
+    <t>ADBE</t>
   </si>
   <si>
-    <t>SONY</t>
-  </si>
-  <si>
-    <t>NIO</t>
-  </si>
-  <si>
-    <t>META</t>
-  </si>
-  <si>
-    <t>NVDA</t>
-  </si>
-  <si>
-    <t>TSLA</t>
+    <t/>
   </si>
 </sst>
 </file>
@@ -52,7 +40,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -102,7 +90,7 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -429,30 +417,22 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="A4" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A5" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="A6" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>